<commit_message>
Activity Rule for trip:
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-erp/src/main/resources/plugin/erp/oob/rule/process.oa.trip/activity-rule.xlsx
+++ b/vertx-pin/zero-erp/src/main/resources/plugin/erp/oob/rule/process.oa.trip/activity-rule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/Develop/Source/ox-workshop/vertx-zero/vertx-pin/zero-erp/src/main/resources/plugin/erp/oob/rule/process.oa.trip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15FE049-5C26-4541-96B6-371139D0E704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA106F1B-33D4-A84F-AB3E-3A5D0BA696C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="56580" yWindow="-5380" windowWidth="57600" windowHeight="26380" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="54720" yWindow="-3240" windowWidth="57600" windowHeight="26380" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-CDATA" sheetId="7" r:id="rId1"/>
@@ -899,7 +899,7 @@
   <dimension ref="A2:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -910,12 +910,12 @@
     <col min="4" max="4" width="17" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="90.1640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="90.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="69.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="99.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="81.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="22.33203125" style="2" bestFit="1" customWidth="1"/>
@@ -967,22 +967,22 @@
         <v>10</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>14</v>
@@ -1017,22 +1017,22 @@
         <v>18</v>
       </c>
       <c r="G4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>22</v>
@@ -1067,22 +1067,22 @@
         <v>32</v>
       </c>
       <c r="G5" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="J5" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="K5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="11" t="b">
+      <c r="L5" s="11" t="b">
         <v>1</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>39</v>
       </c>
       <c r="M5" s="11"/>
       <c r="N5" s="12" t="s">
@@ -1111,22 +1111,22 @@
         <v>46</v>
       </c>
       <c r="G6" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="J6" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="K6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="11" t="b">
+      <c r="L6" s="11" t="b">
         <v>1</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="M6" s="11"/>
       <c r="N6" s="12" t="s">
@@ -1155,22 +1155,22 @@
         <v>48</v>
       </c>
       <c r="G7" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="J7" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="K7" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="11" t="b">
+      <c r="L7" s="11" t="b">
         <v>1</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>51</v>
       </c>
       <c r="M7" s="11"/>
       <c r="N7" s="12" t="s">
@@ -1199,22 +1199,22 @@
         <v>62</v>
       </c>
       <c r="G8" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="J8" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="K8" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="11" t="b">
+      <c r="L8" s="11" t="b">
         <v>1</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>61</v>
       </c>
       <c r="M8" s="11"/>
       <c r="N8" s="12" t="s">
@@ -1243,22 +1243,22 @@
         <v>63</v>
       </c>
       <c r="G9" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="J9" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="K9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J9" s="11" t="b">
+      <c r="L9" s="11" t="b">
         <v>1</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>64</v>
       </c>
       <c r="M9" s="11"/>
       <c r="N9" s="12" t="s">
@@ -1287,22 +1287,22 @@
         <v>85</v>
       </c>
       <c r="G10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="J10" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="K10" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="J10" s="11" t="b">
+      <c r="L10" s="11" t="b">
         <v>1</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>58</v>
       </c>
       <c r="M10" s="11"/>
       <c r="N10" s="12" t="s">
@@ -1331,22 +1331,22 @@
         <v>42</v>
       </c>
       <c r="G11" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="J11" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="K11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="11" t="b">
+      <c r="L11" s="11" t="b">
         <v>1</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="L11" s="11" t="s">
-        <v>56</v>
       </c>
       <c r="M11" s="11"/>
       <c r="N11" s="12" t="s">
@@ -1375,22 +1375,22 @@
         <v>52</v>
       </c>
       <c r="G12" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="J12" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="K12" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="J12" s="11" t="b">
+      <c r="L12" s="11" t="b">
         <v>1</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="L12" s="11" t="s">
-        <v>57</v>
       </c>
       <c r="M12" s="11"/>
       <c r="N12" s="12" t="s">
@@ -1418,23 +1418,23 @@
       <c r="F13" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="J13" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="K13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="11" t="b">
+      <c r="L13" s="11" t="b">
         <v>1</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>60</v>
       </c>
       <c r="M13" s="11"/>
       <c r="N13" s="12" t="s">
@@ -1463,22 +1463,22 @@
         <v>79</v>
       </c>
       <c r="G14" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="J14" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="K14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="11" t="b">
+      <c r="L14" s="11" t="b">
         <v>1</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="L14" s="11" t="s">
-        <v>58</v>
       </c>
       <c r="M14" s="11"/>
       <c r="N14" s="12" t="s">
@@ -1507,22 +1507,22 @@
         <v>42</v>
       </c>
       <c r="G15" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="J15" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="K15" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J15" s="11" t="b">
+      <c r="L15" s="11" t="b">
         <v>1</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>56</v>
       </c>
       <c r="M15" s="11"/>
       <c r="N15" s="12" t="s">
@@ -1551,22 +1551,22 @@
         <v>52</v>
       </c>
       <c r="G16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="J16" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="K16" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="J16" s="11" t="b">
+      <c r="L16" s="11" t="b">
         <v>1</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="L16" s="11" t="s">
-        <v>57</v>
       </c>
       <c r="M16" s="11"/>
       <c r="N16" s="12" t="s">
@@ -1594,23 +1594,23 @@
       <c r="F17" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="I17" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="J17" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="K17" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J17" s="11" t="b">
+      <c r="L17" s="11" t="b">
         <v>1</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="L17" s="11" t="s">
-        <v>89</v>
       </c>
       <c r="M17" s="11"/>
       <c r="N17" s="12" t="s">

</xml_diff>